<commit_message>
started making classification trees and bayes classifier
</commit_message>
<xml_diff>
--- a/workingData.xlsx
+++ b/workingData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79E200C9-A1D6-1F47-9E51-058C44E95C08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD0C363-4788-CC4F-A74A-9C6D34E0C6F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="4040" windowWidth="19620" windowHeight="11440" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="96">
   <si>
     <t>Grocery Store Name</t>
   </si>
@@ -253,13 +253,79 @@
   </si>
   <si>
     <t>Population of Zipcode</t>
+  </si>
+  <si>
+    <t>"97212"</t>
+  </si>
+  <si>
+    <t>"97213"</t>
+  </si>
+  <si>
+    <t>"97214"</t>
+  </si>
+  <si>
+    <t>"97209"</t>
+  </si>
+  <si>
+    <t>"97203"</t>
+  </si>
+  <si>
+    <t>"97217"</t>
+  </si>
+  <si>
+    <t>"97210"</t>
+  </si>
+  <si>
+    <t>"97211"</t>
+  </si>
+  <si>
+    <t>"97232"</t>
+  </si>
+  <si>
+    <t>"97202"</t>
+  </si>
+  <si>
+    <t>"97206"</t>
+  </si>
+  <si>
+    <t>"97266"</t>
+  </si>
+  <si>
+    <t>"97060"</t>
+  </si>
+  <si>
+    <t>"97220"</t>
+  </si>
+  <si>
+    <t>"97030"</t>
+  </si>
+  <si>
+    <t>"97201"</t>
+  </si>
+  <si>
+    <t>"97219"</t>
+  </si>
+  <si>
+    <t>"97236"</t>
+  </si>
+  <si>
+    <t>"97080"</t>
+  </si>
+  <si>
+    <t>"97205"</t>
+  </si>
+  <si>
+    <t>"97216"</t>
+  </si>
+  <si>
+    <t>"97024"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,8 +363,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,22 +681,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="50" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,17 +709,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -663,8 +729,8 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>97212</v>
+      <c r="D2" t="s">
+        <v>74</v>
       </c>
       <c r="E2" s="1">
         <v>76461.512400000007</v>
@@ -676,7 +742,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -686,8 +752,8 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>97213</v>
+      <c r="D3" t="s">
+        <v>75</v>
       </c>
       <c r="E3" s="1">
         <v>59037.809399999998</v>
@@ -699,7 +765,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -709,8 +775,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>97214</v>
+      <c r="D4" t="s">
+        <v>76</v>
       </c>
       <c r="E4" s="1">
         <v>48004.493499999997</v>
@@ -722,7 +788,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -732,8 +798,8 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>97209</v>
+      <c r="D5" t="s">
+        <v>77</v>
       </c>
       <c r="E5" s="1">
         <v>34518.406000000003</v>
@@ -745,7 +811,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -755,8 +821,8 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
-        <v>97203</v>
+      <c r="D6" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="1">
         <v>43918.490100000003</v>
@@ -768,7 +834,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -778,8 +844,8 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
-        <v>97217</v>
+      <c r="D7" t="s">
+        <v>79</v>
       </c>
       <c r="E7" s="1">
         <v>48621.962599999999</v>
@@ -791,7 +857,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -801,8 +867,8 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
-        <v>97210</v>
+      <c r="D8" t="s">
+        <v>80</v>
       </c>
       <c r="E8" s="1">
         <v>61295.774100000002</v>
@@ -814,7 +880,7 @@
         <v>9915</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -824,8 +890,8 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>97212</v>
+      <c r="D9" t="s">
+        <v>74</v>
       </c>
       <c r="E9" s="1">
         <v>76461.512400000007</v>
@@ -837,7 +903,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -847,8 +913,8 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>97211</v>
+      <c r="D10" t="s">
+        <v>81</v>
       </c>
       <c r="E10" s="1">
         <v>55036.634899999997</v>
@@ -860,7 +926,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -870,8 +936,8 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>97232</v>
+      <c r="D11" t="s">
+        <v>82</v>
       </c>
       <c r="E11" s="2">
         <v>55155</v>
@@ -883,7 +949,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -893,8 +959,8 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
-        <v>97214</v>
+      <c r="D12" t="s">
+        <v>76</v>
       </c>
       <c r="E12" s="1">
         <v>48004.493499999997</v>
@@ -906,7 +972,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -916,8 +982,8 @@
       <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
-        <v>97202</v>
+      <c r="D13" t="s">
+        <v>83</v>
       </c>
       <c r="E13" s="1">
         <v>52559.811500000003</v>
@@ -929,7 +995,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -939,8 +1005,8 @@
       <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="D14">
-        <v>97206</v>
+      <c r="D14" t="s">
+        <v>84</v>
       </c>
       <c r="E14" s="1">
         <v>48476.457799999996</v>
@@ -952,7 +1018,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -962,8 +1028,8 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D15">
-        <v>97202</v>
+      <c r="D15" t="s">
+        <v>83</v>
       </c>
       <c r="E15" s="1">
         <v>52559.811500000003</v>
@@ -975,7 +1041,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -985,8 +1051,8 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D16">
-        <v>97217</v>
+      <c r="D16" t="s">
+        <v>79</v>
       </c>
       <c r="E16" s="1">
         <v>48621.962599999999</v>
@@ -998,7 +1064,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1008,8 +1074,8 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17">
-        <v>97266</v>
+      <c r="D17" t="s">
+        <v>85</v>
       </c>
       <c r="E17" s="1">
         <v>41273.908300000003</v>
@@ -1021,7 +1087,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1031,8 +1097,8 @@
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18">
-        <v>97060</v>
+      <c r="D18" t="s">
+        <v>86</v>
       </c>
       <c r="E18" s="1">
         <v>60353.151899999997</v>
@@ -1044,7 +1110,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1054,8 +1120,8 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="D19">
-        <v>97203</v>
+      <c r="D19" t="s">
+        <v>78</v>
       </c>
       <c r="E19" s="1">
         <v>43918.490100000003</v>
@@ -1067,7 +1133,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1077,8 +1143,8 @@
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D20">
-        <v>97213</v>
+      <c r="D20" t="s">
+        <v>75</v>
       </c>
       <c r="E20" s="1">
         <v>59037.809399999998</v>
@@ -1090,7 +1156,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1100,8 +1166,8 @@
       <c r="C21" t="s">
         <v>29</v>
       </c>
-      <c r="D21">
-        <v>97206</v>
+      <c r="D21" t="s">
+        <v>84</v>
       </c>
       <c r="E21" s="1">
         <v>48476.457799999996</v>
@@ -1113,7 +1179,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1123,8 +1189,8 @@
       <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="D22">
-        <v>97266</v>
+      <c r="D22" t="s">
+        <v>85</v>
       </c>
       <c r="E22" s="1">
         <v>41273.908300000003</v>
@@ -1136,7 +1202,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1146,8 +1212,8 @@
       <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="D23">
-        <v>97220</v>
+      <c r="D23" t="s">
+        <v>87</v>
       </c>
       <c r="E23" s="1">
         <v>43212.265700000004</v>
@@ -1159,7 +1225,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1169,8 +1235,8 @@
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="D24">
-        <v>97030</v>
+      <c r="D24" t="s">
+        <v>88</v>
       </c>
       <c r="E24" s="1">
         <v>45355.138500000001</v>
@@ -1182,7 +1248,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1192,8 +1258,8 @@
       <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="D25">
-        <v>97217</v>
+      <c r="D25" t="s">
+        <v>79</v>
       </c>
       <c r="E25" s="1">
         <v>48621.962599999999</v>
@@ -1205,7 +1271,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1215,8 +1281,8 @@
       <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="D26">
-        <v>97201</v>
+      <c r="D26" t="s">
+        <v>89</v>
       </c>
       <c r="E26" s="1">
         <v>51689.527900000001</v>
@@ -1228,7 +1294,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1238,8 +1304,8 @@
       <c r="C27" t="s">
         <v>37</v>
       </c>
-      <c r="D27">
-        <v>97232</v>
+      <c r="D27" t="s">
+        <v>82</v>
       </c>
       <c r="E27" s="1">
         <v>55155.441299999999</v>
@@ -1251,7 +1317,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1261,8 +1327,8 @@
       <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="D28">
-        <v>97203</v>
+      <c r="D28" t="s">
+        <v>78</v>
       </c>
       <c r="E28" s="1">
         <v>43918.490100000003</v>
@@ -1274,7 +1340,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1284,8 +1350,8 @@
       <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="D29">
-        <v>97217</v>
+      <c r="D29" t="s">
+        <v>79</v>
       </c>
       <c r="E29" s="1">
         <v>48621.962599999999</v>
@@ -1297,7 +1363,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1307,8 +1373,8 @@
       <c r="C30" t="s">
         <v>41</v>
       </c>
-      <c r="D30">
-        <v>97209</v>
+      <c r="D30" t="s">
+        <v>77</v>
       </c>
       <c r="E30" s="1">
         <v>34518.406000000003</v>
@@ -1320,7 +1386,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1330,8 +1396,8 @@
       <c r="C31" t="s">
         <v>42</v>
       </c>
-      <c r="D31">
-        <v>97232</v>
+      <c r="D31" t="s">
+        <v>82</v>
       </c>
       <c r="E31" s="1">
         <v>55155.441299999999</v>
@@ -1343,7 +1409,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1353,8 +1419,8 @@
       <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="D32">
-        <v>97219</v>
+      <c r="D32" t="s">
+        <v>90</v>
       </c>
       <c r="E32" s="1">
         <v>78979.374500000005</v>
@@ -1366,7 +1432,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1376,8 +1442,8 @@
       <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="D33">
-        <v>97214</v>
+      <c r="D33" t="s">
+        <v>76</v>
       </c>
       <c r="E33" s="1">
         <v>48004.493499999997</v>
@@ -1389,7 +1455,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1399,8 +1465,8 @@
       <c r="C34" t="s">
         <v>45</v>
       </c>
-      <c r="D34">
-        <v>97213</v>
+      <c r="D34" t="s">
+        <v>75</v>
       </c>
       <c r="E34" s="1">
         <v>59037.809399999998</v>
@@ -1412,7 +1478,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1422,8 +1488,8 @@
       <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="D35">
-        <v>97220</v>
+      <c r="D35" t="s">
+        <v>87</v>
       </c>
       <c r="E35" s="1">
         <v>43212.265700000004</v>
@@ -1435,7 +1501,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1445,8 +1511,8 @@
       <c r="C36" t="s">
         <v>47</v>
       </c>
-      <c r="D36">
-        <v>97236</v>
+      <c r="D36" t="s">
+        <v>91</v>
       </c>
       <c r="E36" s="1">
         <v>47869.868799999997</v>
@@ -1458,7 +1524,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1468,8 +1534,8 @@
       <c r="C37" t="s">
         <v>48</v>
       </c>
-      <c r="D37">
-        <v>97060</v>
+      <c r="D37" t="s">
+        <v>86</v>
       </c>
       <c r="E37" s="1">
         <v>60353.151899999997</v>
@@ -1481,7 +1547,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1491,8 +1557,8 @@
       <c r="C38" t="s">
         <v>50</v>
       </c>
-      <c r="D38">
-        <v>97203</v>
+      <c r="D38" t="s">
+        <v>78</v>
       </c>
       <c r="E38" s="1">
         <v>43918.490100000003</v>
@@ -1504,7 +1570,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1514,8 +1580,8 @@
       <c r="C39" t="s">
         <v>51</v>
       </c>
-      <c r="D39">
-        <v>97211</v>
+      <c r="D39" t="s">
+        <v>81</v>
       </c>
       <c r="E39" s="1">
         <v>55036.634899999997</v>
@@ -1527,7 +1593,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -1537,8 +1603,8 @@
       <c r="C40" t="s">
         <v>52</v>
       </c>
-      <c r="D40">
-        <v>97213</v>
+      <c r="D40" t="s">
+        <v>75</v>
       </c>
       <c r="E40" s="1">
         <v>59037.809399999998</v>
@@ -1550,7 +1616,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1560,8 +1626,8 @@
       <c r="C41" t="s">
         <v>53</v>
       </c>
-      <c r="D41">
-        <v>97232</v>
+      <c r="D41" t="s">
+        <v>82</v>
       </c>
       <c r="E41" s="1">
         <v>55155.441299999999</v>
@@ -1573,7 +1639,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -1583,8 +1649,8 @@
       <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="D42">
-        <v>97209</v>
+      <c r="D42" t="s">
+        <v>77</v>
       </c>
       <c r="E42" s="1">
         <v>34518.406000000003</v>
@@ -1596,7 +1662,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1606,8 +1672,8 @@
       <c r="C43" t="s">
         <v>55</v>
       </c>
-      <c r="D43">
-        <v>97201</v>
+      <c r="D43" t="s">
+        <v>89</v>
       </c>
       <c r="E43" s="1">
         <v>51689.527900000001</v>
@@ -1619,7 +1685,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1629,8 +1695,8 @@
       <c r="C44" t="s">
         <v>56</v>
       </c>
-      <c r="D44">
-        <v>97214</v>
+      <c r="D44" t="s">
+        <v>76</v>
       </c>
       <c r="E44" s="1">
         <v>48004.493499999997</v>
@@ -1642,7 +1708,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1652,8 +1718,8 @@
       <c r="C45" t="s">
         <v>57</v>
       </c>
-      <c r="D45">
-        <v>97202</v>
+      <c r="D45" t="s">
+        <v>83</v>
       </c>
       <c r="E45" s="1">
         <v>52559.811500000003</v>
@@ -1665,7 +1731,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1675,8 +1741,8 @@
       <c r="C46" t="s">
         <v>58</v>
       </c>
-      <c r="D46">
-        <v>97206</v>
+      <c r="D46" t="s">
+        <v>84</v>
       </c>
       <c r="E46" s="1">
         <v>48476.457799999996</v>
@@ -1688,7 +1754,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -1698,8 +1764,8 @@
       <c r="C47" t="s">
         <v>59</v>
       </c>
-      <c r="D47">
-        <v>97219</v>
+      <c r="D47" t="s">
+        <v>90</v>
       </c>
       <c r="E47" s="1">
         <v>78979.374500000005</v>
@@ -1711,7 +1777,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1721,8 +1787,8 @@
       <c r="C48" t="s">
         <v>60</v>
       </c>
-      <c r="D48">
-        <v>97236</v>
+      <c r="D48" t="s">
+        <v>91</v>
       </c>
       <c r="E48" s="1">
         <v>47869.868799999997</v>
@@ -1734,7 +1800,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1744,8 +1810,8 @@
       <c r="C49" t="s">
         <v>61</v>
       </c>
-      <c r="D49">
-        <v>97080</v>
+      <c r="D49" t="s">
+        <v>92</v>
       </c>
       <c r="E49" s="1">
         <v>62759.8413</v>
@@ -1757,7 +1823,7 @@
         <v>33590</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1767,8 +1833,8 @@
       <c r="C50" t="s">
         <v>62</v>
       </c>
-      <c r="D50">
-        <v>97030</v>
+      <c r="D50" t="s">
+        <v>88</v>
       </c>
       <c r="E50" s="1">
         <v>45355.138500000001</v>
@@ -1780,7 +1846,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1790,8 +1856,8 @@
       <c r="C51" t="s">
         <v>63</v>
       </c>
-      <c r="D51">
-        <v>97060</v>
+      <c r="D51" t="s">
+        <v>86</v>
       </c>
       <c r="E51" s="1">
         <v>60353.151899999997</v>
@@ -1803,7 +1869,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -1813,8 +1879,8 @@
       <c r="C52" t="s">
         <v>65</v>
       </c>
-      <c r="D52">
-        <v>97217</v>
+      <c r="D52" t="s">
+        <v>79</v>
       </c>
       <c r="E52" s="1">
         <v>48621.962599999999</v>
@@ -1826,7 +1892,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -1836,8 +1902,8 @@
       <c r="C53" t="s">
         <v>66</v>
       </c>
-      <c r="D53">
-        <v>97205</v>
+      <c r="D53" t="s">
+        <v>93</v>
       </c>
       <c r="E53" s="2">
         <v>40051</v>
@@ -1849,7 +1915,7 @@
         <v>6682</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1859,8 +1925,8 @@
       <c r="C54" t="s">
         <v>67</v>
       </c>
-      <c r="D54">
-        <v>97220</v>
+      <c r="D54" t="s">
+        <v>87</v>
       </c>
       <c r="E54" s="1">
         <v>43212.265700000004</v>
@@ -1872,7 +1938,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -1882,8 +1948,8 @@
       <c r="C55" t="s">
         <v>68</v>
       </c>
-      <c r="D55">
-        <v>97202</v>
+      <c r="D55" t="s">
+        <v>83</v>
       </c>
       <c r="E55" s="1">
         <v>52559.811500000003</v>
@@ -1895,7 +1961,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1905,8 +1971,8 @@
       <c r="C56" t="s">
         <v>69</v>
       </c>
-      <c r="D56">
-        <v>97216</v>
+      <c r="D56" t="s">
+        <v>94</v>
       </c>
       <c r="E56" s="1">
         <v>43895.758099999999</v>
@@ -1918,7 +1984,7 @@
         <v>13563</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1928,8 +1994,8 @@
       <c r="C57" t="s">
         <v>70</v>
       </c>
-      <c r="D57">
-        <v>97024</v>
+      <c r="D57" t="s">
+        <v>95</v>
       </c>
       <c r="E57" s="1">
         <v>51056.430999999997</v>

</xml_diff>

<commit_message>
tried making K-means models a lil more cleaner
</commit_message>
<xml_diff>
--- a/workingData.xlsx
+++ b/workingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD0C363-4788-CC4F-A74A-9C6D34E0C6F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CA0C5-4C47-E645-84BE-88068BE979BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t>Grocery Store Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Whole Foods Market</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>3535 NE 15th Ave, Portland, OR 97212</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Walmart</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>1123 N Hayden Meadows Dr, Portland, OR 97217</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
   </si>
   <si>
     <t>Green Zebra</t>
-  </si>
-  <si>
-    <t>Medium</t>
   </si>
   <si>
     <t>3011 N Lombard St, Portland, OR 97217</t>
@@ -681,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,27 +701,27 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1">
         <v>76461.512400000007</v>
@@ -746,14 +737,14 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3" s="1">
         <v>59037.809399999998</v>
@@ -769,14 +760,14 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1">
         <v>48004.493499999997</v>
@@ -792,14 +783,14 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="1">
         <v>34518.406000000003</v>
@@ -813,16 +804,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1">
         <v>43918.490100000003</v>
@@ -836,16 +827,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E7" s="1">
         <v>48621.962599999999</v>
@@ -859,16 +850,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1">
         <v>61295.774100000002</v>
@@ -882,16 +873,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1">
         <v>76461.512400000007</v>
@@ -905,16 +896,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1">
         <v>55036.634899999997</v>
@@ -928,16 +919,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E11" s="2">
         <v>55155</v>
@@ -951,16 +942,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="1">
         <v>48004.493499999997</v>
@@ -974,16 +965,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1">
         <v>52559.811500000003</v>
@@ -997,16 +988,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E14" s="1">
         <v>48476.457799999996</v>
@@ -1020,16 +1011,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1">
         <v>52559.811500000003</v>
@@ -1043,16 +1034,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1">
         <v>48621.962599999999</v>
@@ -1066,16 +1057,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E17" s="1">
         <v>41273.908300000003</v>
@@ -1089,16 +1080,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E18" s="1">
         <v>60353.151899999997</v>
@@ -1112,16 +1103,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E19" s="1">
         <v>43918.490100000003</v>
@@ -1135,16 +1126,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1">
         <v>59037.809399999998</v>
@@ -1158,16 +1149,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E21" s="1">
         <v>48476.457799999996</v>
@@ -1181,16 +1172,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1">
         <v>41273.908300000003</v>
@@ -1204,16 +1195,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E23" s="1">
         <v>43212.265700000004</v>
@@ -1227,16 +1218,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1">
         <v>45355.138500000001</v>
@@ -1250,16 +1241,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1">
         <v>48621.962599999999</v>
@@ -1273,16 +1264,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1">
         <v>51689.527900000001</v>
@@ -1296,16 +1287,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="1">
         <v>55155.441299999999</v>
@@ -1319,16 +1310,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E28" s="1">
         <v>43918.490100000003</v>
@@ -1342,16 +1333,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E29" s="1">
         <v>48621.962599999999</v>
@@ -1365,16 +1356,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
         <v>38</v>
       </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" t="s">
-        <v>41</v>
-      </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E30" s="1">
         <v>34518.406000000003</v>
@@ -1388,16 +1379,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E31" s="1">
         <v>55155.441299999999</v>
@@ -1411,16 +1402,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E32" s="1">
         <v>78979.374500000005</v>
@@ -1434,16 +1425,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1">
         <v>48004.493499999997</v>
@@ -1457,16 +1448,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E34" s="1">
         <v>59037.809399999998</v>
@@ -1480,16 +1471,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E35" s="1">
         <v>43212.265700000004</v>
@@ -1503,16 +1494,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E36" s="1">
         <v>47869.868799999997</v>
@@ -1526,16 +1517,16 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E37" s="1">
         <v>60353.151899999997</v>
@@ -1549,16 +1540,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E38" s="1">
         <v>43918.490100000003</v>
@@ -1572,16 +1563,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E39" s="1">
         <v>55036.634899999997</v>
@@ -1595,16 +1586,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
         <v>49</v>
       </c>
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" t="s">
-        <v>52</v>
-      </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E40" s="1">
         <v>59037.809399999998</v>
@@ -1618,16 +1609,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E41" s="1">
         <v>55155.441299999999</v>
@@ -1641,16 +1632,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E42" s="1">
         <v>34518.406000000003</v>
@@ -1664,16 +1655,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E43" s="1">
         <v>51689.527900000001</v>
@@ -1687,16 +1678,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E44" s="1">
         <v>48004.493499999997</v>
@@ -1710,16 +1701,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E45" s="1">
         <v>52559.811500000003</v>
@@ -1733,16 +1724,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E46" s="1">
         <v>48476.457799999996</v>
@@ -1756,16 +1747,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E47" s="1">
         <v>78979.374500000005</v>
@@ -1779,16 +1770,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E48" s="1">
         <v>47869.868799999997</v>
@@ -1802,16 +1793,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E49" s="1">
         <v>62759.8413</v>
@@ -1825,16 +1816,16 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E50" s="1">
         <v>45355.138500000001</v>
@@ -1848,16 +1839,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E51" s="1">
         <v>60353.151899999997</v>
@@ -1871,16 +1862,16 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D52" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E52" s="1">
         <v>48621.962599999999</v>
@@ -1894,16 +1885,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E53" s="2">
         <v>40051</v>
@@ -1917,16 +1908,16 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
         <v>64</v>
       </c>
-      <c r="B54" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
-      </c>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E54" s="1">
         <v>43212.265700000004</v>
@@ -1940,16 +1931,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E55" s="1">
         <v>52559.811500000003</v>
@@ -1963,16 +1954,16 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E56" s="1">
         <v>43895.758099999999</v>
@@ -1986,16 +1977,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E57" s="1">
         <v>51056.430999999997</v>

</xml_diff>